<commit_message>
legobot functions and data updates
</commit_message>
<xml_diff>
--- a/Legobot/legobot_turn_data.xlsx
+++ b/Legobot/legobot_turn_data.xlsx
@@ -15,7 +15,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Power 90</t>
+  </si>
   <si>
     <t>Power 80</t>
   </si>
@@ -41,6 +44,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -126,10 +130,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="M10" activeCellId="0" pane="topLeft" sqref="M10"/>
+      <selection activeCell="C5" activeCellId="0" pane="topLeft" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -153,13 +157,34 @@
       <c r="E1" s="0" t="n">
         <v>-30</v>
       </c>
+      <c r="H1" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="I1" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="J1" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="K1" s="0" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="2">
       <c r="B2" s="0" t="n">
-        <v>-180</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>-89.5</v>
+        <v>-177</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>181.2</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>88.3</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>43.2</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>26.6</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="4">
@@ -178,87 +203,124 @@
       <c r="E4" s="0" t="n">
         <v>-30</v>
       </c>
-      <c r="F4" s="0" t="n">
-        <v>-10</v>
-      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="5">
       <c r="B5" s="0" t="n">
-        <v>-180</v>
+        <v>-179</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>-89</v>
+        <v>-86.4</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>-41.5</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>-26.7</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>-7.8</v>
+        <v>-41</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="9">
-      <c r="A9" s="0" t="s">
+      <c r="B7" s="0" t="n">
+        <v>-180</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>-90</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>-45</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>-30</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="8">
+      <c r="E8" s="0" t="n">
+        <v>-26.2</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>181.2</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>88.4</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="10">
+      <c r="A10" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="0" t="n">
-        <v>-180</v>
-      </c>
-      <c r="C9" s="0" t="n">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="13">
+      <c r="A13" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>-180</v>
+      </c>
+      <c r="C13" s="0" t="n">
         <v>-90</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D13" s="0" t="n">
         <v>-45</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E13" s="0" t="n">
         <v>-30</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F13" s="0" t="n">
         <v>-10</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H13" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="I13" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="J9" s="0" t="n">
+      <c r="J13" s="0" t="n">
         <v>45</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="10">
-      <c r="B10" s="0" t="n">
-        <v>-180</v>
-      </c>
-      <c r="C10" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="14">
+      <c r="B14" s="0" t="n">
+        <v>-180</v>
+      </c>
+      <c r="C14" s="0" t="n">
         <v>-88.7</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D14" s="0" t="n">
         <v>-41.9</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E14" s="0" t="n">
         <v>-26.1</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F14" s="0" t="n">
         <v>-7.32</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H14" s="0" t="n">
         <v>183</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="I14" s="0" t="n">
         <v>91.2</v>
       </c>
-      <c r="J10" s="0" t="n">
+      <c r="J14" s="0" t="n">
         <v>43.5</v>
       </c>
-      <c r="M10" s="1"/>
+      <c r="M14" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
create and legobot updates
</commit_message>
<xml_diff>
--- a/Legobot/legobot_turn_data.xlsx
+++ b/Legobot/legobot_turn_data.xlsx
@@ -39,7 +39,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -60,11 +60,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,7 +109,7 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -142,7 +137,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G34" activeCellId="0" pane="topLeft" sqref="G34"/>
+      <selection activeCell="F41" activeCellId="0" pane="topLeft" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -230,6 +225,9 @@
       <c r="J4" s="0" t="n">
         <v>45</v>
       </c>
+      <c r="K4" s="0" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="5">
       <c r="B5" s="0" t="n">
@@ -249,6 +247,12 @@
       </c>
       <c r="I5" s="0" t="n">
         <v>88.36</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>42.9</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>26.7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="7">

</xml_diff>

<commit_message>
minor changes to both
</commit_message>
<xml_diff>
--- a/Legobot/legobot_turn_data.xlsx
+++ b/Legobot/legobot_turn_data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Power 90</t>
   </si>
@@ -30,6 +30,9 @@
   </si>
   <si>
     <t>Power 50</t>
+  </si>
+  <si>
+    <t> data= {{70, -180, -179.6}, {70, -90, -87.75}, {70,-45,-41.8}, {70,-30,-26.2},{70, 180, 181.2}, {70, 90, 88.4}, {70, 45, 42.5}, {70, 30, 29.6},{90, -180, -177.2}, {90, -90, -88.3}, {90, -45, -40.4}, {90, -30, 25.9}, {90, 180, 181.2}, {90, 90, 88.3}, {90, 45, 43.2}, {90, 30, 26.2}, {80, -180, -179}, {80, -90, -86.4}, {80, -45, -42.1}, {80, -30, -26.6},{80, 180, 181.6}, {80, 90, 88.36}, {80, 45, 42.9}, {80, 30, 26.7}, {50, -180, -180}, {50, -90, -88.7}, {50, -45, -41.9}, {50, -30, 26.1}, {50, 180, 183}, {50, 90, 91.2}, {50, 45, 43.5}};</t>
   </si>
 </sst>
 </file>
@@ -134,10 +137,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F41" activeCellId="0" pane="topLeft" sqref="F41"/>
+      <selection activeCell="B26" activeCellId="0" pane="topLeft" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -371,6 +374,11 @@
       </c>
       <c r="M14" s="2"/>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="22">
+      <c r="B22" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>